<commit_message>
Change .Err to .err
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/FAR TAS W16-08.xlsx
+++ b/Tests/Validation/Wheat/data/FAR TAS W16-08.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Wheat\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://faraustralia-my.sharepoint.com/personal/ben_jones_faraustralia_com_au/Documents/Repos/bj-far.ApsimX/Tests/Validation/Wheat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F74D29-4CB0-493C-B91A-3C446FC98217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{60F74D29-4CB0-493C-B91A-3C446FC98217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EA0F96F-A6E2-439C-86C0-59A951DA35B6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$Z$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -508,13 +511,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="G139" sqref="G139"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -594,7 +601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -614,7 +621,7 @@
         <v>21.898796580329901</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -628,7 +635,7 @@
         <v>5.1538820320220701E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -642,7 +649,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -656,7 +663,7 @@
         <v>2.3935677693908502E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -676,7 +683,7 @@
         <v>69.823997486537493</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -690,7 +697,7 @@
         <v>4.0824829046386202E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -704,7 +711,7 @@
         <v>1.6007810593582101E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -718,7 +725,7 @@
         <v>8.5391256382996508E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -738,7 +745,7 @@
         <v>1.7103050525955401</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -752,7 +759,7 @@
         <v>1.19023807142381E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -763,7 +770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -777,7 +784,7 @@
         <v>1.47196014438798E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -791,7 +798,7 @@
         <v>1.2583057392117901E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -805,7 +812,7 @@
         <v>1.25267267907276</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -819,7 +826,7 @@
         <v>1.2583057392117901E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -833,7 +840,7 @@
         <v>1.43614066163451E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -850,7 +857,7 @@
         <v>35.370067382840297</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -891,7 +898,7 @@
         <v>0.23628367735349901</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -911,7 +918,7 @@
         <v>4.8412291827592702</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -925,7 +932,7 @@
         <v>2.1053008494433E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -939,7 +946,7 @@
         <v>6.2915286960589503E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -953,7 +960,7 @@
         <v>8.2600948339995803E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -973,7 +980,7 @@
         <v>19.4186336628851</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -987,7 +994,7 @@
         <v>5.0000000000000096E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>8.1649658092772595E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1029,7 +1036,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1040,7 +1047,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>4.0824829046386202E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1068,7 +1075,7 @@
         <v>2.8867513459481398E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>6.6143782776614604E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1096,7 +1103,7 @@
         <v>9.6824583655185491E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>26.867731575255799</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>0.12689129299622201</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1174,7 +1181,7 @@
         <v>12.8036046356745</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1188,7 +1195,7 @@
         <v>3.1449364063522799E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1223,7 @@
         <v>1.10867789130417E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>29.913068492995901</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1257,7 @@
         <v>4.7871355387816899E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1278,7 +1285,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1303,7 +1310,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -1317,7 +1324,7 @@
         <v>7.5000000000000101E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>1.9148542155126801E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>6.4549722436790299E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>2.1360009363293801E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>6.5351613088992098</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>5.0148953888316798E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -1431,7 +1438,7 @@
         <v>2.2302372818454399E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -1445,7 +1452,7 @@
         <v>4.3301270189222097E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -1459,7 +1466,7 @@
         <v>7.7728158775740097E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -1473,7 +1480,7 @@
         <v>1.31497781983829E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -1501,7 +1508,7 @@
         <v>4.7871355387816899E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -1521,7 +1528,7 @@
         <v>0.62058113824003003</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -1535,7 +1542,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -1546,7 +1553,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -1574,7 +1581,7 @@
         <v>1.22474487139159E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -1588,7 +1595,7 @@
         <v>1.2207782564104099</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -1602,7 +1609,7 @@
         <v>4.7324236215002397E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -1616,7 +1623,7 @@
         <v>1.4790199457749001E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -1633,7 +1640,7 @@
         <v>2.9755951785595198</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>0.167139644087096</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1695,7 @@
         <v>9.4372930440884406E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>1.25000000000001E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -1716,7 +1723,7 @@
         <v>2.3935677693908402E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>30</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>4.7871355387816899E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>4.7871355387817099E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -1758,7 +1765,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>1.3754387954301801</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
@@ -1792,7 +1799,7 @@
         <v>6.2915286960589598E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -1803,7 +1810,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -1817,7 +1824,7 @@
         <v>8.6602540378443605E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -1831,7 +1838,7 @@
         <v>1.31497781983829E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -1845,7 +1852,7 @@
         <v>0.68579435998493399</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>7.35980072193986E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1880,7 @@
         <v>1.06066017177982E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -1890,7 +1897,7 @@
         <v>40.0390434451174</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -1931,7 +1938,7 @@
         <v>0.11703201086562701</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -1945,7 +1952,7 @@
         <v>7.1807033081725501E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -1959,7 +1966,7 @@
         <v>1.4433756729740599E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -1973,7 +1980,7 @@
         <v>3.1457643480294699E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>31</v>
       </c>
@@ -1987,7 +1994,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>31</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>8.6602540378443605E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>31</v>
       </c>
@@ -2015,7 +2022,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>31</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>1.2615156556657601</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>31</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>4.7871355387816899E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>31</v>
       </c>
@@ -2060,7 +2067,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -2074,7 +2081,7 @@
         <v>7.0710678118654701E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -2088,7 +2095,7 @@
         <v>4.7871355387817003E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>31</v>
       </c>
@@ -2102,7 +2109,7 @@
         <v>1.9077461116983101</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -2116,7 +2123,7 @@
         <v>7.3598007219398704E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -2130,7 +2137,7 @@
         <v>8.2915619758885204E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>31</v>
       </c>
@@ -2147,7 +2154,7 @@
         <v>9.2421137553411796</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>31</v>
       </c>
@@ -2188,7 +2195,7 @@
         <v>0.21640927893825701</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>32</v>
       </c>
@@ -2202,7 +2209,7 @@
         <v>1.13651514141549E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>32</v>
       </c>
@@ -2216,7 +2223,7 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>32</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>32</v>
       </c>
@@ -2244,7 +2251,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>32</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>32</v>
       </c>
@@ -2272,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>32</v>
       </c>
@@ -2292,7 +2299,7 @@
         <v>1.25965247179795</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>32</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>32</v>
       </c>
@@ -2317,7 +2324,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>32</v>
       </c>
@@ -2331,7 +2338,7 @@
         <v>4.7871355387817099E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>32</v>
       </c>
@@ -2345,7 +2352,7 @@
         <v>1.5545631755148E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>32</v>
       </c>
@@ -2359,7 +2366,7 @@
         <v>1.49249523407082</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>32</v>
       </c>
@@ -2373,7 +2380,7 @@
         <v>7.4651970279870604E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>32</v>
       </c>
@@ -2387,7 +2394,7 @@
         <v>5.9511903571190404E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>32</v>
       </c>
@@ -2404,7 +2411,7 @@
         <v>23.7719197093265</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>32</v>
       </c>
@@ -2445,7 +2452,7 @@
         <v>0.149171270960024</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -2459,7 +2466,7 @@
         <v>5.1538820320220996E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -2473,7 +2480,7 @@
         <v>2.0412414523193301E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>33</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>3.2274861218395102E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>33</v>
       </c>
@@ -2501,7 +2508,7 @@
         <v>2.8867513459481398E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -2515,7 +2522,7 @@
         <v>4.7871355387817099E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>33</v>
       </c>
@@ -2529,7 +2536,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>33</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v>0.78837561474647799</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>33</v>
       </c>
@@ -2563,7 +2570,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -2574,7 +2581,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>33</v>
       </c>
@@ -2588,7 +2595,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>33</v>
       </c>
@@ -2602,7 +2609,7 @@
         <v>1.9364916731037098E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -2616,7 +2623,7 @@
         <v>1.0591195322131699</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -2630,7 +2637,7 @@
         <v>0.17649805239718699</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>33</v>
       </c>
@@ -2644,7 +2651,7 @@
         <v>4.7871355387817099E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>33</v>
       </c>
@@ -2661,7 +2668,7 @@
         <v>13.9707656077492</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>33</v>
       </c>
@@ -2702,7 +2709,7 @@
         <v>0.22517952404132099</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>34</v>
       </c>
@@ -2716,7 +2723,7 @@
         <v>5.40061724867322E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>34</v>
       </c>
@@ -2730,7 +2737,7 @@
         <v>1.25000000000001E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>34</v>
       </c>
@@ -2744,7 +2751,7 @@
         <v>4.5643546458763902E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>34</v>
       </c>
@@ -2758,7 +2765,7 @@
         <v>6.2915286960589702E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>34</v>
       </c>
@@ -2772,7 +2779,7 @@
         <v>1.03077640640441E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -2786,7 +2793,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -2806,7 +2813,7 @@
         <v>1.15845773390722</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -2820,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>34</v>
       </c>
@@ -2831,7 +2838,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>34</v>
       </c>
@@ -2845,7 +2852,7 @@
         <v>6.4549722436790299E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>34</v>
       </c>
@@ -2859,7 +2866,7 @@
         <v>1.0307764064044199E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>34</v>
       </c>
@@ -2873,7 +2880,7 @@
         <v>1.3095448456126</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>34</v>
       </c>
@@ -2887,7 +2894,7 @@
         <v>2.3837557900646299E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>34</v>
       </c>
@@ -2901,7 +2908,7 @@
         <v>1.9418633662885001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +2925,7 @@
         <v>8.1888516695973106</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>34</v>
       </c>
@@ -2959,7 +2966,7 @@
         <v>0.17964971758096601</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>35</v>
       </c>
@@ -2973,7 +2980,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -2987,7 +2994,7 @@
         <v>2.0412414523193301E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>35</v>
       </c>
@@ -3001,7 +3008,7 @@
         <v>3.2274861218395201E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>35</v>
       </c>
@@ -3015,7 +3022,7 @@
         <v>1.19023807142381E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>35</v>
       </c>
@@ -3029,7 +3036,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3043,7 +3050,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>35</v>
       </c>
@@ -3057,7 +3064,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>35</v>
       </c>
@@ -3068,7 +3075,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>35</v>
       </c>
@@ -3082,7 +3089,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>35</v>
       </c>
@@ -3096,7 +3103,7 @@
         <v>1.6007810593582101E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>35</v>
       </c>
@@ -3110,7 +3117,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>35</v>
       </c>
@@ -3124,7 +3131,7 @@
         <v>1.5991534218662899E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>35</v>
       </c>
@@ -3141,7 +3148,7 @@
         <v>17.245168405479099</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>35</v>
       </c>
@@ -3182,7 +3189,7 @@
         <v>0.16868198701136999</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>36</v>
       </c>
@@ -3196,7 +3203,7 @@
         <v>1.0507933510765399E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>36</v>
       </c>
@@ -3210,7 +3217,7 @@
         <v>4.2695628191498202E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>36</v>
       </c>
@@ -3224,7 +3231,7 @@
         <v>3.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>36</v>
       </c>
@@ -3238,7 +3245,7 @@
         <v>2.8867513459481299E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>36</v>
       </c>
@@ -3252,7 +3259,7 @@
         <v>3.9024564913226999E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>36</v>
       </c>
@@ -3266,7 +3273,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>36</v>
       </c>
@@ -3280,7 +3287,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -3291,7 +3298,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -3305,7 +3312,7 @@
         <v>6.2915286960589399E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -3319,7 +3326,7 @@
         <v>1.31497781983829E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>36</v>
       </c>
@@ -3333,7 +3340,7 @@
         <v>8.5391256382996508E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>36</v>
       </c>
@@ -3347,7 +3354,7 @@
         <v>7.7728158775740097E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>36</v>
       </c>
@@ -3364,7 +3371,7 @@
         <v>10.231690964840601</v>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>36</v>
       </c>
@@ -3405,7 +3412,7 @@
         <v>5.4171086654265801E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>37</v>
       </c>
@@ -3419,7 +3426,7 @@
         <v>5.2041649986653404E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>37</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>1.44337567297405E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>37</v>
       </c>
@@ -3447,7 +3454,7 @@
         <v>2.3935677693908502E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>37</v>
       </c>
@@ -3461,7 +3468,7 @@
         <v>4.7871355387817099E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>37</v>
       </c>
@@ -3475,7 +3482,7 @@
         <v>1.0307764064044199E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>37</v>
       </c>
@@ -3489,7 +3496,7 @@
         <v>7.4999999999999902E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>37</v>
       </c>
@@ -3503,7 +3510,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>37</v>
       </c>
@@ -3514,7 +3521,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>37</v>
       </c>
@@ -3528,7 +3535,7 @@
         <v>8.6602540378443605E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>37</v>
       </c>
@@ -3542,7 +3549,7 @@
         <v>1.5545631755148E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>37</v>
       </c>
@@ -3556,7 +3563,7 @@
         <v>6.5748890991914602E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>37</v>
       </c>
@@ -3570,7 +3577,7 @@
         <v>1.2808688457449501E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>37</v>
       </c>
@@ -3587,7 +3594,7 @@
         <v>11.427990126585399</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>37</v>
       </c>
@@ -3628,7 +3635,7 @@
         <v>0.128033460982347</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>38</v>
       </c>
@@ -3642,7 +3649,7 @@
         <v>3.5355339059327299E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>38</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>8.0039052967910695E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>38</v>
       </c>
@@ -3670,7 +3677,7 @@
         <v>1.44337567297405E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>38</v>
       </c>
@@ -3684,7 +3691,7 @@
         <v>2.8867513459481398E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>38</v>
       </c>
@@ -3698,7 +3705,7 @@
         <v>4.0824829046386298E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>38</v>
       </c>
@@ -3712,7 +3719,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>38</v>
       </c>
@@ -3726,7 +3733,7 @@
         <v>2.4999999999999901E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>38</v>
       </c>
@@ -3737,7 +3744,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>38</v>
       </c>
@@ -3751,7 +3758,7 @@
         <v>2.8867513459481398E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>38</v>
       </c>
@@ -3765,7 +3772,7 @@
         <v>1.6583123951776999E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>38</v>
       </c>
@@ -3779,7 +3786,7 @@
         <v>4.3301270189221698E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>38</v>
       </c>
@@ -3793,7 +3800,7 @@
         <v>1.22474487139159E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>38</v>
       </c>
@@ -3810,7 +3817,7 @@
         <v>5.0518148554092299</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>38</v>
       </c>
@@ -3852,6 +3859,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>